<commit_message>
he hecho el indice del markdown
</commit_message>
<xml_diff>
--- a/data/población_cyl.xlsx
+++ b/data/población_cyl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\seminario_fuentes\Seminario_Fuentes_Datos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95C83FE-BAB4-4BF7-8A6C-B0E475B9B50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9711F437-328B-44CB-A2AB-4B4C5764765D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="14820" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t/>
   </si>
@@ -49,12 +49,6 @@
     <t>Ávila</t>
   </si>
   <si>
-    <t>159.764</t>
-  </si>
-  <si>
-    <t>12.868</t>
-  </si>
-  <si>
     <t>8,05</t>
   </si>
   <si>
@@ -64,12 +58,6 @@
     <t>Burgos</t>
   </si>
   <si>
-    <t>357.370</t>
-  </si>
-  <si>
-    <t>33.150</t>
-  </si>
-  <si>
     <t>9,27</t>
   </si>
   <si>
@@ -79,12 +67,6 @@
     <t>León</t>
   </si>
   <si>
-    <t>448.573</t>
-  </si>
-  <si>
-    <t>23.398</t>
-  </si>
-  <si>
     <t>5,21</t>
   </si>
   <si>
@@ -94,12 +76,6 @@
     <t>Palencia</t>
   </si>
   <si>
-    <t>157.787</t>
-  </si>
-  <si>
-    <t>8.581</t>
-  </si>
-  <si>
     <t>5,43</t>
   </si>
   <si>
@@ -109,12 +85,6 @@
     <t>Salamanca</t>
   </si>
   <si>
-    <t>327.089</t>
-  </si>
-  <si>
-    <t>18.606</t>
-  </si>
-  <si>
     <t>5,68</t>
   </si>
   <si>
@@ -124,12 +94,6 @@
     <t>Segovia</t>
   </si>
   <si>
-    <t>155.332</t>
-  </si>
-  <si>
-    <t>20.015</t>
-  </si>
-  <si>
     <t>12,88</t>
   </si>
   <si>
@@ -139,12 +103,6 @@
     <t>Soria</t>
   </si>
   <si>
-    <t>89.528</t>
-  </si>
-  <si>
-    <t>10.363</t>
-  </si>
-  <si>
     <t>11,57</t>
   </si>
   <si>
@@ -154,12 +112,6 @@
     <t>Valladolid</t>
   </si>
   <si>
-    <t>521.333</t>
-  </si>
-  <si>
-    <t>33.352</t>
-  </si>
-  <si>
     <t>6,39</t>
   </si>
   <si>
@@ -169,12 +121,6 @@
     <t>Zamora</t>
   </si>
   <si>
-    <t>166.927</t>
-  </si>
-  <si>
-    <t>7.601</t>
-  </si>
-  <si>
     <t>4,55</t>
   </si>
   <si>
@@ -182,12 +128,6 @@
   </si>
   <si>
     <t>Castilla y León</t>
-  </si>
-  <si>
-    <t>2.383.703</t>
-  </si>
-  <si>
-    <t>167.934</t>
   </si>
   <si>
     <t>7,04</t>
@@ -229,9 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,12 +510,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="5" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -615,170 +558,170 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>159764</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12868</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>357370</v>
+      </c>
+      <c r="C4" s="2">
+        <v>33150</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>448573</v>
+      </c>
+      <c r="C5" s="2">
+        <v>23398</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>157787</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8581</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>327089</v>
+      </c>
+      <c r="C7" s="2">
+        <v>18606</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <v>155332</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20015</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
+        <v>89528</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10363</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="1">
+        <v>521333</v>
+      </c>
+      <c r="C10" s="2">
+        <v>33352</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
+      </c>
+      <c r="B11" s="1">
+        <v>166927</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7601</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2383703</v>
+      </c>
+      <c r="C12" s="2">
+        <v>167934</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>